<commit_message>
Final tidy of carbon study and add pion decay class and tsts
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/Proton-to-carbon-equivalent-solenoid.xlsx
+++ b/21-Spreads4Tests/Proton-to-carbon-equivalent-solenoid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://api.box.com/wopi/files/2056263865509/WOPIServiceId_TP_BOX_2/WOPIUserId_-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="153" documentId="13_ncr:1_{8D7310F1-EDAC-1446-B06E-D6D217703B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCEA12D9-D978-CB41-B540-B0C79185CE45}"/>
+  <xr:revisionPtr revIDLastSave="166" documentId="13_ncr:1_{8D7310F1-EDAC-1446-B06E-D6D217703B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D37DAB7-D1BC-DC4A-861C-B9BA76A707C4}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{18B04D0A-E0CC-0944-8399-8D7F9F02DB42}"/>
+    <workbookView xWindow="4620" yWindow="5220" windowWidth="25620" windowHeight="14420" xr2:uid="{18B04D0A-E0CC-0944-8399-8D7F9F02DB42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1017,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D62AF3-1C90-7849-BF2D-377057E3DBCC}">
-  <dimension ref="A3:L27"/>
+  <dimension ref="A3:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1031,7 +1031,7 @@
     <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="19" x14ac:dyDescent="0.2">
       <c r="F3" s="41" t="s">
         <v>10</v>
       </c>
@@ -1043,7 +1043,7 @@
       <c r="K3" s="42"/>
       <c r="L3" s="43"/>
     </row>
-    <row r="4" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>10</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>0</v>
       </c>
@@ -1099,7 +1099,7 @@
       </c>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <f>2.4916949087545</f>
         <v>2.4916949087544999</v>
@@ -1136,8 +1136,11 @@
       <c r="L6" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>45.609479836855826</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <f>1.01874726126505</f>
         <v>1.0187472612650501</v>
@@ -1175,7 +1178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <f>1.4485646330252</f>
         <v>1.4485646330252</v>
@@ -1213,7 +1216,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <f>1.78885896627796</f>
         <v>1.7888589662779599</v>
@@ -1245,7 +1248,7 @@
       </c>
       <c r="L9" s="9"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <f>1.60433994066042</f>
         <v>1.60433994066042</v>
@@ -1263,7 +1266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <f>1.24481401652751</f>
         <v>1.2448140165275099</v>
@@ -1296,7 +1299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
         <v>1.1659674900000001</v>
       </c>
@@ -1313,7 +1316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="20" x14ac:dyDescent="0.25">
       <c r="F13" s="21" t="s">
         <v>25</v>
       </c>
@@ -1330,8 +1333,9 @@
         <v>9.0073371204394598E-2</v>
       </c>
       <c r="L13" s="24"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N13" s="35"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -1348,8 +1352,11 @@
       <c r="J14" s="26"/>
       <c r="K14" s="37"/>
       <c r="L14" s="27"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N14">
+        <v>1.9617360767163099</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -1375,7 +1382,7 @@
       </c>
       <c r="L15" s="30"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>9</v>
       </c>
@@ -1400,13 +1407,13 @@
         <v>1.961736076716311</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="J20">
         <f>G13/K13</f>
         <v>1.9617360770365053</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>23</v>
       </c>
@@ -1422,7 +1429,7 @@
         <v>3.0448809512810553</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>24</v>
       </c>
@@ -1434,7 +1441,7 @@
         <v>4.9698511972451342E-10</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C26">
         <f>(C23-C24)/C23</f>
         <v>-6.8008910925431029E-11</v>
@@ -1444,10 +1451,15 @@
         <v>1.961736076716311</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
       <c r="J27">
         <f>J26-J20</f>
         <v>-3.2019431550622812E-10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L30">
+        <v>1.9617360767163099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>